<commit_message>
test : vietnamese io
</commit_message>
<xml_diff>
--- a/Goods.xlsx
+++ b/Goods.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d5c0a0a63df9b95f/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\New Course\PBL2\PBL2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="317" documentId="8_{97F26CBB-47EC-47AE-A158-08C328C8C9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE08501C-5491-4C4D-A822-CC7917AA9930}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFE9707-102C-4716-A774-54BBEF8D0325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8B3122E1-B9EE-4EBD-A591-496BE62D3DB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8B3122E1-B9EE-4EBD-A591-496BE62D3DB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -558,7 +558,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -581,51 +581,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -633,16 +599,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -961,30 +918,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A2B384-B17D-4AE2-A3A5-1C77290F3EB2}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="62" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:A42"/>
+    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6:O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="15.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.08984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.90625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="8.7265625" style="1"/>
-    <col min="11" max="11" width="12.54296875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="28.54296875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="25" style="1" customWidth="1"/>
-    <col min="14" max="14" width="36.7265625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="43.26953125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.77734375" style="5"/>
+    <col min="2" max="2" width="15.77734375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18" style="5" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="5" customWidth="1"/>
+    <col min="9" max="10" width="8.77734375" style="5"/>
+    <col min="11" max="11" width="12.5546875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="28.5546875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="25" style="5" customWidth="1"/>
+    <col min="14" max="14" width="36.77734375" style="5" customWidth="1"/>
+    <col min="15" max="15" width="43.21875" style="5" customWidth="1"/>
+    <col min="16" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1030,819 +987,850 @@
       <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="109.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:16" ht="109.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" ht="27.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="3" t="s">
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" ht="27.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" ht="14.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="1:16" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="3" t="s">
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" ht="64.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="O6" s="2"/>
-    </row>
-    <row r="7" spans="1:16" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="3" t="s">
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" ht="64.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2" t="s">
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2" t="s">
+      <c r="J9" s="3"/>
+      <c r="K9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="3" t="s">
+      <c r="L9" s="3"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="3" t="s">
+      <c r="N10" s="3"/>
+      <c r="O10" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="113.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="3" t="s">
+    <row r="11" spans="1:16" ht="113.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-    </row>
-    <row r="14" spans="1:16" ht="86" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:16" ht="85.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
       <c r="I14" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="N14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="O14" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="86" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+    <row r="15" spans="1:16" ht="85.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="J15" s="1"/>
       <c r="K15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-    </row>
-    <row r="16" spans="1:16" ht="86" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:16" ht="85.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
       <c r="I16" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="J16" s="1"/>
       <c r="K16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="1:15" ht="218" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="1:15" ht="217.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
       <c r="I17" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="J17" s="1"/>
       <c r="K17" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="M17" s="1"/>
+      <c r="N17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="O17" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="218" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+    <row r="18" spans="1:15" ht="217.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
       <c r="I18" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="J18" s="1"/>
       <c r="K18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-    </row>
-    <row r="19" spans="1:15" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="L18" s="3"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
       <c r="I19" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="J19" s="1"/>
       <c r="K19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="L19" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
       <c r="I20" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="J20" s="1"/>
       <c r="K20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
       <c r="I21" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:15" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="L21" s="3"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" ht="159.44999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
       <c r="I22" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="L22" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="M22" s="4" t="s">
+      <c r="M22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N22" s="2" t="s">
+      <c r="N22" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="O22" s="2" t="s">
+      <c r="O22" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
       <c r="I23" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="J23" s="1"/>
       <c r="K23" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="L23" s="2"/>
+      <c r="L23" s="3"/>
       <c r="M23" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
       <c r="I24" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="J24" s="1"/>
       <c r="K24" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="L24" s="2"/>
+      <c r="L24" s="3"/>
       <c r="M24" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
       <c r="I25" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="J25" s="1"/>
       <c r="K25" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-    </row>
-    <row r="26" spans="1:15" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+      <c r="L25" s="3"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="1:15" ht="72.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
       <c r="I26" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="J26" s="1"/>
       <c r="K26" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="L26" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5" t="s">
+      <c r="M26" s="1"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
       <c r="I27" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="J27" s="1"/>
       <c r="K27" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="L27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
       <c r="I28" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="J28" s="1"/>
       <c r="K28" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-    </row>
-    <row r="29" spans="1:15" ht="87" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
+      <c r="L28" s="3"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="1:15" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5" t="s">
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5" t="s">
+      <c r="J29" s="3"/>
+      <c r="K29" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="L29" s="3" t="s">
         <v>106</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="N29" s="5" t="s">
+      <c r="N29" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="O29" s="5" t="s">
+      <c r="O29" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
       <c r="M30" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
       <c r="M31" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-    </row>
-    <row r="33" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+    </row>
+    <row r="33" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5" t="s">
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5" t="s">
+      <c r="J33" s="3"/>
+      <c r="K33" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="L33" s="3" t="s">
         <v>118</v>
       </c>
       <c r="M33" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N33" s="5" t="s">
+      <c r="N33" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="O33" s="5" t="s">
+      <c r="O33" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
       <c r="M34" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
       <c r="M35" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
       <c r="M36" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
-    </row>
-    <row r="37" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+    </row>
+    <row r="37" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>121</v>
       </c>
@@ -1858,15 +1846,20 @@
       <c r="E37" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
         <v>123</v>
       </c>
+      <c r="J37" s="1"/>
       <c r="K37" s="1" t="s">
         <v>124</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="M37" s="1"/>
       <c r="N37" s="1" t="s">
         <v>126</v>
       </c>
@@ -1874,7 +1867,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>128</v>
       </c>
@@ -1890,15 +1883,20 @@
       <c r="E38" s="1" t="s">
         <v>130</v>
       </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
       <c r="I38" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="J38" s="1"/>
       <c r="K38" s="1" t="s">
         <v>132</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="M38" s="1"/>
       <c r="N38" s="1" t="s">
         <v>135</v>
       </c>
@@ -1906,239 +1904,203 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="116" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
+    <row r="39" spans="1:15" ht="115.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
       <c r="I39" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5" t="s">
+      <c r="J39" s="3"/>
+      <c r="K39" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="L39" s="5" t="s">
+      <c r="L39" s="3" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+    </row>
+    <row r="40" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
       <c r="I40" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-    </row>
-    <row r="41" spans="1:15" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+    </row>
+    <row r="41" spans="1:15" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
       <c r="I41" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5" t="s">
+      <c r="J41" s="3"/>
+      <c r="K41" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="L41" s="5" t="s">
+      <c r="L41" s="3" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+    </row>
+    <row r="42" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
       <c r="I42" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-    </row>
-    <row r="43" spans="1:15" ht="116" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="5" t="s">
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+    </row>
+    <row r="43" spans="1:15" ht="115.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
       <c r="I43" s="1" t="s">
         <v>153</v>
       </c>
+      <c r="J43" s="1"/>
       <c r="K43" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="L43" s="5" t="s">
+      <c r="L43" s="3" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+    </row>
+    <row r="44" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
       <c r="I44" s="1" t="s">
         <v>154</v>
       </c>
+      <c r="J44" s="1"/>
       <c r="K44" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="L44" s="7"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="146">
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="L41:L42"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="K41:K42"/>
-    <mergeCell ref="J39:J40"/>
-    <mergeCell ref="J41:J42"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="L33:L36"/>
-    <mergeCell ref="K33:K36"/>
-    <mergeCell ref="I33:I36"/>
-    <mergeCell ref="J29:J32"/>
-    <mergeCell ref="H33:H36"/>
-    <mergeCell ref="G33:G36"/>
-    <mergeCell ref="F33:F36"/>
-    <mergeCell ref="E33:E36"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="J33:J36"/>
-    <mergeCell ref="N29:N32"/>
-    <mergeCell ref="O29:O32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="N33:N36"/>
-    <mergeCell ref="O33:O36"/>
-    <mergeCell ref="G29:G32"/>
-    <mergeCell ref="H29:H32"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="L29:L32"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="L26:L28"/>
-    <mergeCell ref="O26:O28"/>
-    <mergeCell ref="N26:N28"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="L22:L25"/>
-    <mergeCell ref="N22:N25"/>
-    <mergeCell ref="O22:O25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="M14:M16"/>
-    <mergeCell ref="L14:L16"/>
-    <mergeCell ref="O14:O16"/>
-    <mergeCell ref="N14:N16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="L19:L21"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F2:F13"/>
+    <mergeCell ref="G2:G13"/>
+    <mergeCell ref="H2:H13"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="C2:C13"/>
+    <mergeCell ref="D2:D13"/>
+    <mergeCell ref="E2:E13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="N12:N13"/>
     <mergeCell ref="I2:I8"/>
     <mergeCell ref="J2:J8"/>
     <mergeCell ref="K2:K8"/>
@@ -2155,43 +2117,99 @@
     <mergeCell ref="O10:O11"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="L2:L13"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="C2:C13"/>
-    <mergeCell ref="D2:D13"/>
-    <mergeCell ref="E2:E13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="F2:F13"/>
-    <mergeCell ref="G2:G13"/>
-    <mergeCell ref="H2:H13"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="L19:L21"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="L14:L16"/>
+    <mergeCell ref="O14:O16"/>
+    <mergeCell ref="N14:N16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="L22:L25"/>
+    <mergeCell ref="N22:N25"/>
+    <mergeCell ref="O22:O25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="L26:L28"/>
+    <mergeCell ref="O26:O28"/>
+    <mergeCell ref="N26:N28"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="N29:N32"/>
+    <mergeCell ref="O29:O32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="N33:N36"/>
+    <mergeCell ref="O33:O36"/>
+    <mergeCell ref="G29:G32"/>
+    <mergeCell ref="H29:H32"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="L29:L32"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="L33:L36"/>
+    <mergeCell ref="K33:K36"/>
+    <mergeCell ref="I33:I36"/>
+    <mergeCell ref="J29:J32"/>
+    <mergeCell ref="H33:H36"/>
+    <mergeCell ref="G33:G36"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="J33:J36"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="K41:K42"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="J41:J42"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="L41:L42"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A41:A42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>